<commit_message>
added new capabilities and comments
</commit_message>
<xml_diff>
--- a/src/nlp/data/abbreviations.xlsx
+++ b/src/nlp/data/abbreviations.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mandd/projects/sr2ml/src/nlp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CCFD89-D932-4842-961C-DE7FB933B48C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C308AC83-46DA-6F4E-9900-5AE402D8BB17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54700" yWindow="1640" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40600" yWindow="-420" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="abbreviations" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="914">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="934">
   <si>
     <t>Full</t>
   </si>
@@ -1486,9 +1486,6 @@
     <t>rad</t>
   </si>
   <si>
-    <t>radius</t>
-  </si>
-  <si>
     <t>rd</t>
   </si>
   <si>
@@ -1873,9 +1870,6 @@
     <t>indirect</t>
   </si>
   <si>
-    <t>indicative</t>
-  </si>
-  <si>
     <t>indef</t>
   </si>
   <si>
@@ -2762,6 +2756,72 @@
   </si>
   <si>
     <t>unkwn</t>
+  </si>
+  <si>
+    <t>indicator</t>
+  </si>
+  <si>
+    <t>pck</t>
+  </si>
+  <si>
+    <t>pack</t>
+  </si>
+  <si>
+    <t>security</t>
+  </si>
+  <si>
+    <t>oper</t>
+  </si>
+  <si>
+    <t>operator</t>
+  </si>
+  <si>
+    <t>repck</t>
+  </si>
+  <si>
+    <t>repack</t>
+  </si>
+  <si>
+    <t>radiation</t>
+  </si>
+  <si>
+    <t>refurb</t>
+  </si>
+  <si>
+    <t>refurbish</t>
+  </si>
+  <si>
+    <t>rsvr</t>
+  </si>
+  <si>
+    <t>reservoir</t>
+  </si>
+  <si>
+    <t>resrvr</t>
+  </si>
+  <si>
+    <t>reterm</t>
+  </si>
+  <si>
+    <t>retermination</t>
+  </si>
+  <si>
+    <t>flng</t>
+  </si>
+  <si>
+    <t>flnge</t>
+  </si>
+  <si>
+    <t>ch</t>
+  </si>
+  <si>
+    <t>flngs</t>
+  </si>
+  <si>
+    <t>flanges</t>
+  </si>
+  <si>
+    <t>obsrv</t>
   </si>
 </sst>
 </file>
@@ -3613,11 +3673,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B524"/>
+  <dimension ref="A1:B537"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A198" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A203" sqref="A203"/>
+      <pane ySplit="1" topLeftCell="A523" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A539" sqref="A539"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3652,18 +3712,18 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>527</v>
+      </c>
+      <c r="B4" t="s">
         <v>528</v>
-      </c>
-      <c r="B4" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>529</v>
+      </c>
+      <c r="B5" t="s">
         <v>530</v>
-      </c>
-      <c r="B5" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -3676,7 +3736,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B7" t="s">
         <v>387</v>
@@ -3684,23 +3744,23 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>532</v>
+      </c>
+      <c r="B8" t="s">
         <v>533</v>
-      </c>
-      <c r="B8" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="B9" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -3708,34 +3768,34 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>534</v>
+      </c>
+      <c r="B11" t="s">
         <v>535</v>
-      </c>
-      <c r="B11" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B12" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="B13" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>537</v>
+      </c>
+      <c r="B14" t="s">
         <v>538</v>
-      </c>
-      <c r="B14" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -3743,7 +3803,7 @@
         <v>147</v>
       </c>
       <c r="B15" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -3751,15 +3811,15 @@
         <v>148</v>
       </c>
       <c r="B16" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>539</v>
+      </c>
+      <c r="B17" t="s">
         <v>540</v>
-      </c>
-      <c r="B17" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -3767,7 +3827,7 @@
         <v>423</v>
       </c>
       <c r="B18" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -3780,7 +3840,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -3788,10 +3848,10 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B21" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -3807,15 +3867,15 @@
         <v>276</v>
       </c>
       <c r="B23" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>544</v>
+      </c>
+      <c r="B24" t="s">
         <v>545</v>
-      </c>
-      <c r="B24" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -3831,28 +3891,28 @@
         <v>110</v>
       </c>
       <c r="B26" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="B27" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="B28" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="B29" t="s">
         <v>53</v>
@@ -3876,10 +3936,10 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>547</v>
+      </c>
+      <c r="B32" t="s">
         <v>548</v>
-      </c>
-      <c r="B32" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -3887,23 +3947,23 @@
         <v>424</v>
       </c>
       <c r="B33" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>549</v>
+      </c>
+      <c r="B34" t="s">
         <v>550</v>
-      </c>
-      <c r="B34" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="B35" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -3916,7 +3976,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B37" t="s">
         <v>283</v>
@@ -3932,18 +3992,18 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>552</v>
+      </c>
+      <c r="B39" t="s">
         <v>553</v>
-      </c>
-      <c r="B39" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="B40" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -3972,10 +4032,10 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="B44" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -3988,15 +4048,15 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>554</v>
+      </c>
+      <c r="B46" t="s">
         <v>555</v>
-      </c>
-      <c r="B46" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="B47" t="s">
         <v>11</v>
@@ -4031,7 +4091,7 @@
         <v>149</v>
       </c>
       <c r="B51" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -4044,10 +4104,10 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>557</v>
+      </c>
+      <c r="B53" t="s">
         <v>558</v>
-      </c>
-      <c r="B53" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -4100,7 +4160,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B60" t="s">
         <v>11</v>
@@ -4135,7 +4195,7 @@
         <v>1</v>
       </c>
       <c r="B64" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -4156,7 +4216,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="B67" t="s">
         <v>67</v>
@@ -4164,7 +4224,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="B68" t="s">
         <v>67</v>
@@ -4180,15 +4240,15 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="B70" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="B71" t="s">
         <v>12</v>
@@ -4204,18 +4264,18 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="B73" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="B74" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
@@ -4228,7 +4288,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B76" t="s">
         <v>13</v>
@@ -4247,15 +4307,15 @@
         <v>435</v>
       </c>
       <c r="B78" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>560</v>
+      </c>
+      <c r="B79" t="s">
         <v>561</v>
-      </c>
-      <c r="B79" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
@@ -4268,7 +4328,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="B81" t="s">
         <v>436</v>
@@ -4284,10 +4344,10 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="B83" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
@@ -4295,7 +4355,7 @@
         <v>438</v>
       </c>
       <c r="B84" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
@@ -4303,7 +4363,7 @@
         <v>438</v>
       </c>
       <c r="B85" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
@@ -4311,7 +4371,7 @@
         <v>438</v>
       </c>
       <c r="B86" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
@@ -4324,7 +4384,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B88" t="s">
         <v>14</v>
@@ -4351,7 +4411,7 @@
         <v>246</v>
       </c>
       <c r="B91" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
@@ -4364,7 +4424,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B93" t="s">
         <v>60</v>
@@ -4404,10 +4464,10 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
+        <v>564</v>
+      </c>
+      <c r="B98" t="s">
         <v>565</v>
-      </c>
-      <c r="B98" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
@@ -4428,42 +4488,42 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B101" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>568</v>
+      </c>
+      <c r="B102" t="s">
         <v>569</v>
-      </c>
-      <c r="B102" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B103" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B104" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B105" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
@@ -4479,7 +4539,7 @@
         <v>391</v>
       </c>
       <c r="B107" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
@@ -4487,28 +4547,28 @@
         <v>391</v>
       </c>
       <c r="B108" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="B109" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
+        <v>572</v>
+      </c>
+      <c r="B110" t="s">
         <v>573</v>
-      </c>
-      <c r="B110" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="B111" t="s">
         <v>394</v>
@@ -4516,18 +4576,18 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="B112" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="B113" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
@@ -4564,10 +4624,10 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="B118" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
@@ -4580,7 +4640,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B120" t="s">
         <v>439</v>
@@ -4596,7 +4656,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B122" t="s">
         <v>60</v>
@@ -4604,7 +4664,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B123" t="s">
         <v>247</v>
@@ -4631,28 +4691,28 @@
         <v>445</v>
       </c>
       <c r="B126" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="B127" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
+        <v>510</v>
+      </c>
+      <c r="B128" t="s">
         <v>511</v>
-      </c>
-      <c r="B128" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="B129" t="s">
         <v>15</v>
@@ -4660,7 +4720,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="B130" t="s">
         <v>16</v>
@@ -4668,10 +4728,10 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
+        <v>574</v>
+      </c>
+      <c r="B131" t="s">
         <v>575</v>
-      </c>
-      <c r="B131" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
@@ -4700,18 +4760,18 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
+        <v>504</v>
+      </c>
+      <c r="B135" t="s">
         <v>505</v>
-      </c>
-      <c r="B135" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
@@ -4724,42 +4784,42 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
+        <v>576</v>
+      </c>
+      <c r="B138" t="s">
         <v>577</v>
-      </c>
-      <c r="B138" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="B139" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="B140" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
+        <v>578</v>
+      </c>
+      <c r="B141" t="s">
         <v>579</v>
-      </c>
-      <c r="B141" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="B142" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
@@ -4767,7 +4827,7 @@
         <v>249</v>
       </c>
       <c r="B143" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
@@ -4796,10 +4856,10 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
+        <v>580</v>
+      </c>
+      <c r="B147" t="s">
         <v>581</v>
-      </c>
-      <c r="B147" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
@@ -4820,15 +4880,15 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="B150" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="B151" t="s">
         <v>17</v>
@@ -4855,7 +4915,7 @@
         <v>18</v>
       </c>
       <c r="B154" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
@@ -4863,15 +4923,15 @@
         <v>18</v>
       </c>
       <c r="B155" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B156" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
@@ -4879,7 +4939,7 @@
         <v>404</v>
       </c>
       <c r="B157" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
@@ -4887,7 +4947,7 @@
         <v>405</v>
       </c>
       <c r="B158" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
@@ -4924,34 +4984,34 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
+        <v>583</v>
+      </c>
+      <c r="B163" t="s">
         <v>584</v>
-      </c>
-      <c r="B163" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="B164" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
+        <v>585</v>
+      </c>
+      <c r="B165" t="s">
         <v>586</v>
-      </c>
-      <c r="B165" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="B166" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
@@ -4964,10 +5024,10 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
+        <v>587</v>
+      </c>
+      <c r="B168" t="s">
         <v>588</v>
-      </c>
-      <c r="B168" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
@@ -4991,23 +5051,23 @@
         <v>72</v>
       </c>
       <c r="B171" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
+        <v>590</v>
+      </c>
+      <c r="B172" t="s">
         <v>591</v>
-      </c>
-      <c r="B172" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="B173" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
@@ -5020,23 +5080,23 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
+        <v>592</v>
+      </c>
+      <c r="B175" t="s">
         <v>593</v>
-      </c>
-      <c r="B175" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B176" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="B177" t="s">
         <v>52</v>
@@ -5052,7 +5112,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="B179" t="s">
         <v>309</v>
@@ -5111,7 +5171,7 @@
         <v>410</v>
       </c>
       <c r="B186" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
@@ -5127,7 +5187,7 @@
         <v>221</v>
       </c>
       <c r="B188" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
@@ -5151,7 +5211,7 @@
         <v>222</v>
       </c>
       <c r="B191" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
@@ -5164,10 +5224,10 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
+        <v>595</v>
+      </c>
+      <c r="B193" t="s">
         <v>596</v>
-      </c>
-      <c r="B193" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
@@ -5188,34 +5248,34 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
+        <v>597</v>
+      </c>
+      <c r="B196" t="s">
         <v>598</v>
-      </c>
-      <c r="B196" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
+        <v>599</v>
+      </c>
+      <c r="B197" t="s">
         <v>600</v>
-      </c>
-      <c r="B197" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B198" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
+        <v>602</v>
+      </c>
+      <c r="B199" t="s">
         <v>603</v>
-      </c>
-      <c r="B199" t="s">
-        <v>604</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
@@ -5228,18 +5288,18 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B201" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
+        <v>605</v>
+      </c>
+      <c r="B202" t="s">
         <v>606</v>
-      </c>
-      <c r="B202" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
@@ -5260,10 +5320,10 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B205" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
@@ -5271,7 +5331,7 @@
         <v>253</v>
       </c>
       <c r="B206" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
@@ -5279,7 +5339,7 @@
         <v>254</v>
       </c>
       <c r="B207" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
@@ -5332,7 +5392,7 @@
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="B214" t="s">
         <v>19</v>
@@ -5348,7 +5408,7 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="B216" t="s">
         <v>19</v>
@@ -5388,31 +5448,31 @@
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
+        <v>609</v>
+      </c>
+      <c r="B221" t="s">
         <v>610</v>
-      </c>
-      <c r="B221" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
+        <v>611</v>
+      </c>
+      <c r="B222" t="s">
         <v>612</v>
-      </c>
-      <c r="B222" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B223" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="B224" t="s">
         <v>21</v>
@@ -5420,74 +5480,74 @@
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
+        <v>614</v>
+      </c>
+      <c r="B225" t="s">
         <v>615</v>
-      </c>
-      <c r="B225" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B226" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B227" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B228" t="s">
-        <v>617</v>
+        <v>912</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B229" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B230" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B231" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B232" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B233" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.2">
@@ -5500,18 +5560,18 @@
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B235" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B236" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.2">
@@ -5524,7 +5584,7 @@
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="B238" t="s">
         <v>141</v>
@@ -5532,7 +5592,7 @@
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="B239" t="s">
         <v>141</v>
@@ -5540,10 +5600,10 @@
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B240" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.2">
@@ -5556,18 +5616,18 @@
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B242" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B243" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.2">
@@ -5588,10 +5648,10 @@
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B246" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.2">
@@ -5604,26 +5664,26 @@
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="B248" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B249" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B250" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.2">
@@ -5636,10 +5696,10 @@
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="B252" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.2">
@@ -5668,10 +5728,10 @@
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B256" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.2">
@@ -5719,7 +5779,7 @@
         <v>248</v>
       </c>
       <c r="B262" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.2">
@@ -5748,18 +5808,18 @@
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="B266" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="B267" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.2">
@@ -5772,10 +5832,10 @@
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B269" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.2">
@@ -5812,39 +5872,39 @@
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B274" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B275" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B276" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B277" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B278" t="s">
         <v>22</v>
@@ -5852,10 +5912,10 @@
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B279" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.2">
@@ -5924,7 +5984,7 @@
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="B288" t="s">
         <v>68</v>
@@ -5940,7 +6000,7 @@
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="B290" t="s">
         <v>68</v>
@@ -5956,10 +6016,10 @@
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="B292" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.2">
@@ -5983,7 +6043,7 @@
         <v>195</v>
       </c>
       <c r="B295" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.2">
@@ -6007,12 +6067,12 @@
         <v>472</v>
       </c>
       <c r="B298" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B299" t="s">
         <v>23</v>
@@ -6023,7 +6083,7 @@
         <v>202</v>
       </c>
       <c r="B300" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.2">
@@ -6044,7 +6104,7 @@
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="B303" t="s">
         <v>27</v>
@@ -6076,7 +6136,7 @@
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="B307" t="s">
         <v>198</v>
@@ -6108,7 +6168,7 @@
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="B311" t="s">
         <v>24</v>
@@ -6116,10 +6176,10 @@
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
+        <v>518</v>
+      </c>
+      <c r="B312" t="s">
         <v>519</v>
-      </c>
-      <c r="B312" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.2">
@@ -6127,7 +6187,7 @@
         <v>201</v>
       </c>
       <c r="B313" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.2">
@@ -6156,7 +6216,7 @@
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B317" t="s">
         <v>25</v>
@@ -6164,7 +6224,7 @@
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B318" t="s">
         <v>25</v>
@@ -6172,7 +6232,7 @@
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="B319" t="s">
         <v>26</v>
@@ -6180,10 +6240,10 @@
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B320" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.2">
@@ -6196,15 +6256,15 @@
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="B322" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="B323" t="s">
         <v>29</v>
@@ -6212,26 +6272,26 @@
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
+        <v>664</v>
+      </c>
+      <c r="B324" t="s">
         <v>666</v>
-      </c>
-      <c r="B324" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="B325" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B326" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.2">
@@ -6260,10 +6320,10 @@
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B330" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.2">
@@ -6287,7 +6347,7 @@
         <v>207</v>
       </c>
       <c r="B333" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.2">
@@ -6295,7 +6355,7 @@
         <v>207</v>
       </c>
       <c r="B334" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.2">
@@ -6303,20 +6363,20 @@
         <v>207</v>
       </c>
       <c r="B335" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B336" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="B337" t="s">
         <v>30</v>
@@ -6324,7 +6384,7 @@
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="B338" t="s">
         <v>31</v>
@@ -6332,26 +6392,26 @@
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B339" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
+        <v>673</v>
+      </c>
+      <c r="B340" t="s">
         <v>675</v>
-      </c>
-      <c r="B340" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B341" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.2">
@@ -6375,7 +6435,7 @@
         <v>209</v>
       </c>
       <c r="B344" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.2">
@@ -6388,15 +6448,15 @@
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B346" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="B347" t="s">
         <v>32</v>
@@ -6404,18 +6464,18 @@
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="B348" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B349" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.2">
@@ -6423,7 +6483,7 @@
         <v>210</v>
       </c>
       <c r="B350" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.2">
@@ -6447,7 +6507,7 @@
         <v>231</v>
       </c>
       <c r="B353" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.2">
@@ -6460,10 +6520,10 @@
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="B355" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.2">
@@ -6492,10 +6552,10 @@
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="B359" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.2">
@@ -6516,47 +6576,47 @@
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="B362" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="B363" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="B364" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="B365" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B366" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="B367" t="s">
         <v>33</v>
@@ -6575,7 +6635,7 @@
         <v>96</v>
       </c>
       <c r="B369" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.2">
@@ -6588,10 +6648,10 @@
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B371" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.2">
@@ -6604,7 +6664,7 @@
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="B373" t="s">
         <v>34</v>
@@ -6612,42 +6672,42 @@
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="B374" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="B375" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
+        <v>506</v>
+      </c>
+      <c r="B376" t="s">
         <v>507</v>
-      </c>
-      <c r="B376" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="B377" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="B378" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.2">
@@ -6676,7 +6736,7 @@
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="B382" t="s">
         <v>214</v>
@@ -6695,12 +6755,12 @@
         <v>487</v>
       </c>
       <c r="B384" t="s">
-        <v>488</v>
+        <v>920</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B385" t="s">
         <v>418</v>
@@ -6708,10 +6768,10 @@
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="B386" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.2">
@@ -6732,18 +6792,18 @@
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
+        <v>489</v>
+      </c>
+      <c r="B389" t="s">
         <v>490</v>
-      </c>
-      <c r="B389" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
+        <v>513</v>
+      </c>
+      <c r="B390" t="s">
         <v>514</v>
-      </c>
-      <c r="B390" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.2">
@@ -6756,7 +6816,7 @@
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="B392" t="s">
         <v>79</v>
@@ -6764,18 +6824,18 @@
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
+        <v>700</v>
+      </c>
+      <c r="B393" t="s">
         <v>702</v>
-      </c>
-      <c r="B393" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="B394" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.2">
@@ -6796,7 +6856,7 @@
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="B397" t="s">
         <v>139</v>
@@ -6804,7 +6864,7 @@
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B398" t="s">
         <v>35</v>
@@ -6820,7 +6880,7 @@
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="B400" t="s">
         <v>36</v>
@@ -6828,7 +6888,7 @@
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="B401" t="s">
         <v>36</v>
@@ -6836,7 +6896,7 @@
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B402" t="s">
         <v>81</v>
@@ -6852,15 +6912,15 @@
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B404" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B405" t="s">
         <v>82</v>
@@ -6868,7 +6928,7 @@
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B406" t="s">
         <v>37</v>
@@ -6876,7 +6936,7 @@
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B407" t="s">
         <v>38</v>
@@ -6956,42 +7016,42 @@
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="B417" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
+        <v>708</v>
+      </c>
+      <c r="B418" t="s">
         <v>710</v>
-      </c>
-      <c r="B418" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A419" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="B419" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A420" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="B420" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A421" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="B421" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.2">
@@ -7004,15 +7064,15 @@
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
+        <v>491</v>
+      </c>
+      <c r="B423" t="s">
         <v>492</v>
-      </c>
-      <c r="B423" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B424" t="s">
         <v>356</v>
@@ -7028,7 +7088,7 @@
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A426" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="B426" t="s">
         <v>355</v>
@@ -7047,15 +7107,15 @@
         <v>167</v>
       </c>
       <c r="B428" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
+        <v>493</v>
+      </c>
+      <c r="B429" t="s">
         <v>494</v>
-      </c>
-      <c r="B429" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.2">
@@ -7068,15 +7128,15 @@
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="B431" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A432" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="B432" t="s">
         <v>39</v>
@@ -7084,15 +7144,15 @@
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A433" t="s">
+        <v>495</v>
+      </c>
+      <c r="B433" t="s">
         <v>496</v>
-      </c>
-      <c r="B433" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A434" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="B434" t="s">
         <v>233</v>
@@ -7100,7 +7160,7 @@
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A435" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="B435" t="s">
         <v>40</v>
@@ -7108,7 +7168,7 @@
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A436" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="B436" t="s">
         <v>40</v>
@@ -7124,7 +7184,7 @@
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A438" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="B438" t="s">
         <v>362</v>
@@ -7140,34 +7200,34 @@
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A440" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="B440" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A441" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="B441" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A442" t="s">
+        <v>718</v>
+      </c>
+      <c r="B442" t="s">
         <v>720</v>
-      </c>
-      <c r="B442" t="s">
-        <v>722</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A443" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="B443" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.2">
@@ -7183,12 +7243,12 @@
         <v>55</v>
       </c>
       <c r="B445" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A446" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="B446" t="s">
         <v>56</v>
@@ -7196,26 +7256,26 @@
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A447" t="s">
+        <v>520</v>
+      </c>
+      <c r="B447" t="s">
         <v>521</v>
-      </c>
-      <c r="B447" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A448" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="B448" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A449" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="B449" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.2">
@@ -7231,7 +7291,7 @@
         <v>85</v>
       </c>
       <c r="B451" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.2">
@@ -7239,31 +7299,31 @@
         <v>85</v>
       </c>
       <c r="B452" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A453" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="B453" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A454" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="B454" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
     </row>
     <row r="455" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A455" t="s">
+        <v>724</v>
+      </c>
+      <c r="B455" t="s">
         <v>726</v>
-      </c>
-      <c r="B455" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.2">
@@ -7276,7 +7336,7 @@
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A457" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="B457" t="s">
         <v>41</v>
@@ -7316,7 +7376,7 @@
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A462" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="B462" t="s">
         <v>61</v>
@@ -7324,7 +7384,7 @@
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A463" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="B463" t="s">
         <v>42</v>
@@ -7332,7 +7392,7 @@
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A464" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="B464" t="s">
         <v>45</v>
@@ -7340,15 +7400,15 @@
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A465" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="B465" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A466" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B466" t="s">
         <v>44</v>
@@ -7356,7 +7416,7 @@
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A467" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="B467" t="s">
         <v>44</v>
@@ -7375,31 +7435,31 @@
         <v>106</v>
       </c>
       <c r="B469" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A470" t="s">
+        <v>498</v>
+      </c>
+      <c r="B470" t="s">
         <v>499</v>
-      </c>
-      <c r="B470" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A471" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="B471" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A472" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="B472" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.2">
@@ -7436,39 +7496,39 @@
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A477" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="B477" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="478" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A478" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="B478" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
     </row>
     <row r="479" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A479" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B479" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
     </row>
     <row r="480" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A480" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B480" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="481" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A481" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="B481" t="s">
         <v>46</v>
@@ -7476,15 +7536,15 @@
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A482" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="B482" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
     </row>
     <row r="483" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A483" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B483" t="s">
         <v>47</v>
@@ -7492,7 +7552,7 @@
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A484" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="B484" t="s">
         <v>47</v>
@@ -7500,10 +7560,10 @@
     </row>
     <row r="485" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A485" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="B485" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.2">
@@ -7527,7 +7587,7 @@
         <v>236</v>
       </c>
       <c r="B488" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.2">
@@ -7543,15 +7603,15 @@
         <v>237</v>
       </c>
       <c r="B490" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A491" t="s">
+        <v>500</v>
+      </c>
+      <c r="B491" t="s">
         <v>501</v>
-      </c>
-      <c r="B491" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.2">
@@ -7572,7 +7632,7 @@
     </row>
     <row r="494" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A494" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="B494" t="s">
         <v>48</v>
@@ -7588,7 +7648,7 @@
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A496" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="B496" t="s">
         <v>48</v>
@@ -7599,7 +7659,7 @@
         <v>216</v>
       </c>
       <c r="B497" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.2">
@@ -7620,26 +7680,26 @@
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A500" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="B500" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A501" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="B501" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A502" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="B502" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.2">
@@ -7660,10 +7720,10 @@
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A505" t="s">
+        <v>508</v>
+      </c>
+      <c r="B505" t="s">
         <v>509</v>
-      </c>
-      <c r="B505" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.2">
@@ -7676,7 +7736,7 @@
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A507" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="B507" t="s">
         <v>49</v>
@@ -7684,18 +7744,18 @@
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A508" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="B508" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
     </row>
     <row r="509" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A509" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="B509" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
     </row>
     <row r="510" spans="1:2" x14ac:dyDescent="0.2">
@@ -7727,12 +7787,12 @@
         <v>238</v>
       </c>
       <c r="B513" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
     </row>
     <row r="514" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A514" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="B514" t="s">
         <v>422</v>
@@ -7751,23 +7811,23 @@
         <v>419</v>
       </c>
       <c r="B516" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
     </row>
     <row r="517" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A517" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B517" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
     </row>
     <row r="518" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A518" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B518" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
     </row>
     <row r="519" spans="1:2" x14ac:dyDescent="0.2">
@@ -7796,15 +7856,15 @@
     </row>
     <row r="522" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A522" t="s">
+        <v>502</v>
+      </c>
+      <c r="B522" t="s">
         <v>503</v>
-      </c>
-      <c r="B522" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="523" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A523" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="B523" t="s">
         <v>50</v>
@@ -7812,10 +7872,114 @@
     </row>
     <row r="524" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A524" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B524" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="525" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A525" t="s">
+        <v>913</v>
+      </c>
+      <c r="B525" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="526" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A526" t="s">
+        <v>112</v>
+      </c>
+      <c r="B526" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="527" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A527" t="s">
+        <v>916</v>
+      </c>
+      <c r="B527" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="528" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A528" t="s">
+        <v>918</v>
+      </c>
+      <c r="B528" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="529" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A529" t="s">
+        <v>921</v>
+      </c>
+      <c r="B529" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="530" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A530" t="s">
+        <v>923</v>
+      </c>
+      <c r="B530" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="531" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A531" t="s">
+        <v>925</v>
+      </c>
+      <c r="B531" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="532" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A532" t="s">
+        <v>926</v>
+      </c>
+      <c r="B532" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="533" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A533" t="s">
+        <v>928</v>
+      </c>
+      <c r="B533" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="534" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A534" t="s">
+        <v>929</v>
+      </c>
+      <c r="B534" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="535" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A535" t="s">
+        <v>930</v>
+      </c>
+      <c r="B535" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="536" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A536" t="s">
+        <v>931</v>
+      </c>
+      <c r="B536" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="537" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A537" t="s">
+        <v>933</v>
+      </c>
+      <c r="B537" t="s">
+        <v>660</v>
       </c>
     </row>
   </sheetData>

</xml_diff>